<commit_message>
fix reading lesson with enter to hause
</commit_message>
<xml_diff>
--- a/documents/excel_file.xlsx
+++ b/documents/excel_file.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="Лист1 (engl)" sheetId="3" r:id="rId2"/>
     <sheet name="Лист2" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="114210"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="59">
   <si>
     <t>Дні, числа</t>
   </si>
@@ -208,13 +208,19 @@
   </si>
   <si>
     <t>Інформаційна політика та зв'язки з громадскістю                                         Кульчій І.О.                                                                     103-П</t>
+  </si>
+  <si>
+    <t>використовуйте  основний вхід корпусу А</t>
+  </si>
+  <si>
+    <t>використовуйте  додатковий вхід корпусу П</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -253,11 +259,10 @@
     <font>
       <b/>
       <sz val="24"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -275,7 +280,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor indexed="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -585,6 +590,17 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="medium">
@@ -593,24 +609,13 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
@@ -729,7 +734,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -750,7 +758,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -758,25 +766,17 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -814,9 +814,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -848,10 +848,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -883,10 +882,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1059,23 +1057,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.42578125" customWidth="1"/>
     <col min="2" max="2" width="6.5703125" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" customWidth="1"/>
     <col min="4" max="4" width="49.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" style="48" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1">
       <c r="A1" s="45"/>
     </row>
-    <row r="2" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" ht="29.25" thickBot="1">
       <c r="A2" s="43" t="s">
         <v>0</v>
       </c>
@@ -1089,7 +1090,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="31.5" customHeight="1" thickBot="1">
       <c r="A3" s="43" t="s">
         <v>10</v>
       </c>
@@ -1101,8 +1102,8 @@
       </c>
       <c r="D3" s="46"/>
     </row>
-    <row r="4" spans="1:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="51"/>
+    <row r="4" spans="1:6" ht="33" customHeight="1" thickBot="1">
+      <c r="A4" s="52"/>
       <c r="B4" s="3">
         <v>2</v>
       </c>
@@ -1111,8 +1112,8 @@
       </c>
       <c r="D4" s="46"/>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="52"/>
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A5" s="53"/>
       <c r="B5" s="2">
         <v>3</v>
       </c>
@@ -1121,8 +1122,8 @@
       </c>
       <c r="D5" s="46"/>
     </row>
-    <row r="6" spans="1:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="52"/>
+    <row r="6" spans="1:6" ht="21" customHeight="1" thickBot="1">
+      <c r="A6" s="53"/>
       <c r="B6" s="2">
         <v>4</v>
       </c>
@@ -1131,8 +1132,8 @@
       </c>
       <c r="D6" s="46"/>
     </row>
-    <row r="7" spans="1:6" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="52"/>
+    <row r="7" spans="1:6" ht="17.25" customHeight="1" thickBot="1">
+      <c r="A7" s="53"/>
       <c r="B7" s="2">
         <v>5</v>
       </c>
@@ -1141,8 +1142,8 @@
       </c>
       <c r="D7" s="46"/>
     </row>
-    <row r="8" spans="1:6" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="53"/>
+    <row r="8" spans="1:6" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A8" s="54"/>
       <c r="B8" s="4">
         <v>6</v>
       </c>
@@ -1154,7 +1155,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="34.5" customHeight="1" thickBot="1">
       <c r="A9" s="44" t="s">
         <v>15</v>
       </c>
@@ -1166,8 +1167,8 @@
       </c>
       <c r="D9" s="46"/>
     </row>
-    <row r="10" spans="1:6" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="48" t="s">
+    <row r="10" spans="1:6" ht="31.5" customHeight="1" thickBot="1">
+      <c r="A10" s="49" t="s">
         <v>44</v>
       </c>
       <c r="B10" s="3">
@@ -1179,9 +1180,12 @@
       <c r="D10" s="46" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="49"/>
+      <c r="E10" s="48" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A11" s="50"/>
       <c r="B11" s="2">
         <v>3</v>
       </c>
@@ -1190,8 +1194,8 @@
       </c>
       <c r="D11" s="46"/>
     </row>
-    <row r="12" spans="1:6" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="49"/>
+    <row r="12" spans="1:6" ht="16.5" customHeight="1" thickBot="1">
+      <c r="A12" s="50"/>
       <c r="B12" s="2">
         <v>4</v>
       </c>
@@ -1200,8 +1204,8 @@
       </c>
       <c r="D12" s="46"/>
     </row>
-    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="49"/>
+    <row r="13" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A13" s="50"/>
       <c r="B13" s="2">
         <v>5</v>
       </c>
@@ -1210,8 +1214,8 @@
       </c>
       <c r="D13" s="46"/>
     </row>
-    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="50"/>
+    <row r="14" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A14" s="51"/>
       <c r="B14" s="4">
         <v>6</v>
       </c>
@@ -1220,7 +1224,7 @@
       </c>
       <c r="D14" s="46"/>
     </row>
-    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="15.75" thickBot="1">
       <c r="A15" s="44" t="s">
         <v>16</v>
       </c>
@@ -1234,8 +1238,8 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="48" t="s">
+    <row r="16" spans="1:6" ht="30.75" thickBot="1">
+      <c r="A16" s="49" t="s">
         <v>45</v>
       </c>
       <c r="B16" s="3">
@@ -1248,8 +1252,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="49"/>
+    <row r="17" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A17" s="50"/>
       <c r="B17" s="2">
         <v>3</v>
       </c>
@@ -1258,8 +1262,8 @@
       </c>
       <c r="D17" s="46"/>
     </row>
-    <row r="18" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="49"/>
+    <row r="18" spans="1:5" ht="18" customHeight="1" thickBot="1">
+      <c r="A18" s="50"/>
       <c r="B18" s="2">
         <v>4</v>
       </c>
@@ -1268,8 +1272,8 @@
       </c>
       <c r="D18" s="46"/>
     </row>
-    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="49"/>
+    <row r="19" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A19" s="50"/>
       <c r="B19" s="2">
         <v>5</v>
       </c>
@@ -1278,8 +1282,8 @@
       </c>
       <c r="D19" s="47"/>
     </row>
-    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="50"/>
+    <row r="20" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A20" s="51"/>
       <c r="B20" s="4">
         <v>6</v>
       </c>
@@ -1288,7 +1292,7 @@
       </c>
       <c r="D20" s="46"/>
     </row>
-    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="15.75" thickBot="1">
       <c r="A21" s="44" t="s">
         <v>17</v>
       </c>
@@ -1300,8 +1304,8 @@
       </c>
       <c r="D21" s="46"/>
     </row>
-    <row r="22" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="48" t="s">
+    <row r="22" spans="1:5" ht="45.75" thickBot="1">
+      <c r="A22" s="49" t="s">
         <v>46</v>
       </c>
       <c r="B22" s="3">
@@ -1313,9 +1317,12 @@
       <c r="D22" s="46" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="49"/>
+      <c r="E22" s="48" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="18" customHeight="1" thickBot="1">
+      <c r="A23" s="50"/>
       <c r="B23" s="2">
         <v>3</v>
       </c>
@@ -1324,8 +1331,8 @@
       </c>
       <c r="D23" s="46"/>
     </row>
-    <row r="24" spans="1:4" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="49"/>
+    <row r="24" spans="1:5" ht="16.5" customHeight="1" thickBot="1">
+      <c r="A24" s="50"/>
       <c r="B24" s="2">
         <v>4</v>
       </c>
@@ -1334,8 +1341,8 @@
       </c>
       <c r="D24" s="46"/>
     </row>
-    <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="49"/>
+    <row r="25" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A25" s="50"/>
       <c r="B25" s="2">
         <v>5</v>
       </c>
@@ -1344,8 +1351,8 @@
       </c>
       <c r="D25" s="46"/>
     </row>
-    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="50"/>
+    <row r="26" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A26" s="51"/>
       <c r="B26" s="4">
         <v>6</v>
       </c>
@@ -1354,7 +1361,7 @@
       </c>
       <c r="D26" s="46"/>
     </row>
-    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="15.75" thickBot="1">
       <c r="A27" s="44" t="s">
         <v>18</v>
       </c>
@@ -1366,8 +1373,8 @@
       </c>
       <c r="D27" s="46"/>
     </row>
-    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="48" t="s">
+    <row r="28" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A28" s="49" t="s">
         <v>47</v>
       </c>
       <c r="B28" s="3">
@@ -1378,8 +1385,8 @@
       </c>
       <c r="D28" s="46"/>
     </row>
-    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="49"/>
+    <row r="29" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A29" s="50"/>
       <c r="B29" s="2">
         <v>3</v>
       </c>
@@ -1388,8 +1395,8 @@
       </c>
       <c r="D29" s="46"/>
     </row>
-    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="49"/>
+    <row r="30" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A30" s="50"/>
       <c r="B30" s="2">
         <v>4</v>
       </c>
@@ -1398,8 +1405,8 @@
       </c>
       <c r="D30" s="46"/>
     </row>
-    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="49"/>
+    <row r="31" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A31" s="50"/>
       <c r="B31" s="2">
         <v>5</v>
       </c>
@@ -1408,8 +1415,8 @@
       </c>
       <c r="D31" s="46"/>
     </row>
-    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="50"/>
+    <row r="32" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A32" s="51"/>
       <c r="B32" s="4">
         <v>6</v>
       </c>
@@ -1418,7 +1425,7 @@
       </c>
       <c r="D32" s="46"/>
     </row>
-    <row r="33" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="13.5" customHeight="1">
       <c r="A33" s="6"/>
       <c r="B33" s="38"/>
       <c r="C33" s="39"/>
@@ -1434,7 +1441,7 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="32" max="16383" man="1"/>
   </rowBreaks>
@@ -1442,14 +1449,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L65"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.42578125" customWidth="1"/>
     <col min="2" max="3" width="4.5703125" customWidth="1"/>
@@ -1459,18 +1466,18 @@
     <col min="7" max="7" width="45.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1">
       <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="54" t="s">
+    <row r="2" spans="1:9" ht="29.25" thickBot="1">
+      <c r="A2" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
       <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1481,13 +1488,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="54" t="s">
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A3" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
       <c r="E3" s="2">
         <v>1</v>
       </c>
@@ -1496,7 +1503,7 @@
       </c>
       <c r="G3" s="18"/>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15" customHeight="1" thickBot="1">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -1517,7 +1524,7 @@
       </c>
       <c r="G4" s="18"/>
     </row>
-    <row r="5" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" thickBot="1">
       <c r="A5" s="33">
         <v>9</v>
       </c>
@@ -1538,7 +1545,7 @@
       </c>
       <c r="G5" s="18"/>
     </row>
-    <row r="6" spans="1:9" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="33.75" customHeight="1" thickBot="1">
       <c r="A6" s="26">
         <v>23</v>
       </c>
@@ -1559,7 +1566,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="32.25" customHeight="1" thickBot="1">
       <c r="A7" s="22"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -1574,7 +1581,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="18.75" customHeight="1" thickBot="1">
       <c r="A8" s="7"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -1590,13 +1597,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="54" t="s">
+    <row r="9" spans="1:9" ht="20.25" customHeight="1" thickBot="1">
+      <c r="A9" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="55"/>
-      <c r="C9" s="55"/>
-      <c r="D9" s="55"/>
+      <c r="B9" s="56"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="56"/>
       <c r="E9" s="2">
         <v>1</v>
       </c>
@@ -1607,7 +1614,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="15.75" customHeight="1" thickBot="1">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -1630,7 +1637,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="15.75" thickBot="1">
       <c r="A11" s="33">
         <v>10</v>
       </c>
@@ -1653,7 +1660,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="33.75" customHeight="1" thickBot="1">
       <c r="A12" s="26">
         <v>24</v>
       </c>
@@ -1674,7 +1681,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="30.75" thickBot="1">
       <c r="A13" s="22"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -1689,7 +1696,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="15.75" thickBot="1">
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -1702,13 +1709,13 @@
       </c>
       <c r="G14" s="18"/>
     </row>
-    <row r="15" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="54" t="s">
+    <row r="15" spans="1:9" ht="30.75" thickBot="1">
+      <c r="A15" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="55"/>
-      <c r="C15" s="55"/>
-      <c r="D15" s="55"/>
+      <c r="B15" s="56"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
       <c r="E15" s="2">
         <v>1</v>
       </c>
@@ -1719,7 +1726,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="30.75" thickBot="1">
       <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
@@ -1742,7 +1749,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="30.75" thickBot="1">
       <c r="A17" s="33">
         <v>11</v>
       </c>
@@ -1765,7 +1772,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="33" customHeight="1" thickBot="1">
       <c r="A18" s="26">
         <v>25</v>
       </c>
@@ -1786,7 +1793,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="15.75" thickBot="1">
       <c r="A19" s="22"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -1799,7 +1806,7 @@
       </c>
       <c r="G19" s="19"/>
     </row>
-    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="15.75" thickBot="1">
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -1812,13 +1819,13 @@
       </c>
       <c r="G20" s="18"/>
     </row>
-    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="54" t="s">
+    <row r="21" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A21" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="55"/>
-      <c r="C21" s="55"/>
-      <c r="D21" s="55"/>
+      <c r="B21" s="56"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="56"/>
       <c r="E21" s="2">
         <v>1</v>
       </c>
@@ -1829,7 +1836,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="30.75" thickBot="1">
       <c r="A22" s="2" t="s">
         <v>11</v>
       </c>
@@ -1852,7 +1859,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="18" customHeight="1" thickBot="1">
       <c r="A23" s="33">
         <v>12</v>
       </c>
@@ -1873,7 +1880,7 @@
       </c>
       <c r="G23" s="18"/>
     </row>
-    <row r="24" spans="1:7" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="16.5" customHeight="1" thickBot="1">
       <c r="A24" s="26">
         <v>26</v>
       </c>
@@ -1892,7 +1899,7 @@
       </c>
       <c r="G24" s="18"/>
     </row>
-    <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="15.75" thickBot="1">
       <c r="A25" s="22"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -1905,7 +1912,7 @@
       </c>
       <c r="G25" s="18"/>
     </row>
-    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="15.75" thickBot="1">
       <c r="A26" s="7"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
@@ -1918,13 +1925,13 @@
       </c>
       <c r="G26" s="18"/>
     </row>
-    <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="54" t="s">
+    <row r="27" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A27" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="B27" s="55"/>
-      <c r="C27" s="55"/>
-      <c r="D27" s="56"/>
+      <c r="B27" s="56"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="57"/>
       <c r="E27" s="2">
         <v>1</v>
       </c>
@@ -1933,7 +1940,7 @@
       </c>
       <c r="G27" s="18"/>
     </row>
-    <row r="28" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="30.75" thickBot="1">
       <c r="A28" s="2" t="s">
         <v>11</v>
       </c>
@@ -1956,7 +1963,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="30.75" thickBot="1">
       <c r="A29" s="33">
         <v>13</v>
       </c>
@@ -1979,7 +1986,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="30.75" thickBot="1">
       <c r="A30" s="26">
         <v>27</v>
       </c>
@@ -2000,7 +2007,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="15.75" thickBot="1">
       <c r="A31" s="22"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
@@ -2013,7 +2020,7 @@
       </c>
       <c r="G31" s="18"/>
     </row>
-    <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" ht="15.75" thickBot="1">
       <c r="A32" s="7"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
@@ -2026,7 +2033,7 @@
       </c>
       <c r="G32" s="18"/>
     </row>
-    <row r="33" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="13.5" customHeight="1">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
@@ -2035,18 +2042,18 @@
       <c r="F33" s="39"/>
       <c r="G33" s="40"/>
     </row>
-    <row r="34" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" ht="15.75" thickBot="1">
       <c r="A34" s="42" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="29.25" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="54" t="s">
+    <row r="35" spans="1:10" ht="29.25" thickBot="1">
+      <c r="A35" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B35" s="55"/>
-      <c r="C35" s="55"/>
-      <c r="D35" s="55"/>
+      <c r="B35" s="56"/>
+      <c r="C35" s="56"/>
+      <c r="D35" s="56"/>
       <c r="E35" s="1" t="s">
         <v>1</v>
       </c>
@@ -2057,13 +2064,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="54" t="s">
+    <row r="36" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A36" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="B36" s="55"/>
-      <c r="C36" s="55"/>
-      <c r="D36" s="56"/>
+      <c r="B36" s="56"/>
+      <c r="C36" s="56"/>
+      <c r="D36" s="57"/>
       <c r="E36" s="23">
         <v>1</v>
       </c>
@@ -2072,7 +2079,7 @@
       </c>
       <c r="G36" s="18"/>
     </row>
-    <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" ht="15.75" thickBot="1">
       <c r="A37" s="2" t="s">
         <v>11</v>
       </c>
@@ -2093,7 +2100,7 @@
       </c>
       <c r="G37" s="18"/>
     </row>
-    <row r="38" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" ht="15.75" thickBot="1">
       <c r="A38" s="33">
         <v>16</v>
       </c>
@@ -2114,7 +2121,7 @@
       </c>
       <c r="G38" s="18"/>
     </row>
-    <row r="39" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" ht="30.75" thickBot="1">
       <c r="A39" s="26">
         <v>30</v>
       </c>
@@ -2135,7 +2142,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" ht="15.75" thickBot="1">
       <c r="A40" s="22"/>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
@@ -2148,7 +2155,7 @@
       </c>
       <c r="G40" s="18"/>
     </row>
-    <row r="41" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" ht="15.75" thickBot="1">
       <c r="A41" s="7"/>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
@@ -2161,13 +2168,13 @@
       </c>
       <c r="G41" s="18"/>
     </row>
-    <row r="42" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="54" t="s">
+    <row r="42" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A42" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="B42" s="55"/>
-      <c r="C42" s="55"/>
-      <c r="D42" s="56"/>
+      <c r="B42" s="56"/>
+      <c r="C42" s="56"/>
+      <c r="D42" s="57"/>
       <c r="E42" s="23">
         <v>1</v>
       </c>
@@ -2176,7 +2183,7 @@
       </c>
       <c r="G42" s="18"/>
     </row>
-    <row r="43" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" ht="15.75" thickBot="1">
       <c r="A43" s="2" t="s">
         <v>11</v>
       </c>
@@ -2200,7 +2207,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" ht="15.75" thickBot="1">
       <c r="A44" s="33">
         <v>17</v>
       </c>
@@ -2221,7 +2228,7 @@
       </c>
       <c r="G44" s="18"/>
     </row>
-    <row r="45" spans="1:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" ht="30.75" customHeight="1" thickBot="1">
       <c r="A45" s="26"/>
       <c r="B45" s="20">
         <v>15</v>
@@ -2240,7 +2247,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" ht="30.75" thickBot="1">
       <c r="A46" s="30"/>
       <c r="B46" s="20">
         <v>29</v>
@@ -2257,7 +2264,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" ht="15.75" thickBot="1">
       <c r="A47" s="7"/>
       <c r="B47" s="8"/>
       <c r="C47" s="8"/>
@@ -2270,13 +2277,13 @@
       </c>
       <c r="G47" s="18"/>
     </row>
-    <row r="48" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="54" t="s">
+    <row r="48" spans="1:10" ht="30.75" thickBot="1">
+      <c r="A48" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="B48" s="55"/>
-      <c r="C48" s="55"/>
-      <c r="D48" s="56"/>
+      <c r="B48" s="56"/>
+      <c r="C48" s="56"/>
+      <c r="D48" s="57"/>
       <c r="E48" s="23">
         <v>1</v>
       </c>
@@ -2287,7 +2294,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" ht="30.75" thickBot="1">
       <c r="A49" s="2" t="s">
         <v>11</v>
       </c>
@@ -2310,7 +2317,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" ht="30.75" thickBot="1">
       <c r="A50" s="33">
         <v>18</v>
       </c>
@@ -2333,7 +2340,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" ht="15.75" thickBot="1">
       <c r="A51" s="26"/>
       <c r="B51" s="20">
         <v>16</v>
@@ -2350,7 +2357,7 @@
       </c>
       <c r="G51" s="18"/>
     </row>
-    <row r="52" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" ht="15.75" thickBot="1">
       <c r="A52" s="30"/>
       <c r="B52" s="20">
         <v>30</v>
@@ -2368,7 +2375,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" ht="15.75" thickBot="1">
       <c r="A53" s="7"/>
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
@@ -2381,13 +2388,13 @@
       </c>
       <c r="G53" s="18"/>
     </row>
-    <row r="54" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="54" t="s">
+    <row r="54" spans="1:12" ht="30.75" thickBot="1">
+      <c r="A54" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="B54" s="55"/>
-      <c r="C54" s="55"/>
-      <c r="D54" s="56"/>
+      <c r="B54" s="56"/>
+      <c r="C54" s="56"/>
+      <c r="D54" s="57"/>
       <c r="E54" s="23">
         <v>1</v>
       </c>
@@ -2398,7 +2405,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" ht="30.75" thickBot="1">
       <c r="A55" s="2" t="s">
         <v>11</v>
       </c>
@@ -2421,7 +2428,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" ht="15.75" thickBot="1">
       <c r="A56" s="33">
         <v>19</v>
       </c>
@@ -2442,7 +2449,7 @@
       </c>
       <c r="G56" s="18"/>
     </row>
-    <row r="57" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" ht="15.75" thickBot="1">
       <c r="A57" s="26"/>
       <c r="B57" s="20">
         <v>17</v>
@@ -2459,7 +2466,7 @@
       </c>
       <c r="G57" s="19"/>
     </row>
-    <row r="58" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" ht="15.75" thickBot="1">
       <c r="A58" s="30"/>
       <c r="B58" s="20">
         <v>31</v>
@@ -2474,7 +2481,7 @@
       </c>
       <c r="G58" s="18"/>
     </row>
-    <row r="59" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" ht="15.75" thickBot="1">
       <c r="A59" s="7"/>
       <c r="B59" s="8"/>
       <c r="C59" s="8"/>
@@ -2487,13 +2494,13 @@
       </c>
       <c r="G59" s="18"/>
     </row>
-    <row r="60" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="54" t="s">
+    <row r="60" spans="1:12" ht="30.75" thickBot="1">
+      <c r="A60" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="B60" s="55"/>
-      <c r="C60" s="55"/>
-      <c r="D60" s="56"/>
+      <c r="B60" s="56"/>
+      <c r="C60" s="56"/>
+      <c r="D60" s="57"/>
       <c r="E60" s="2">
         <v>1</v>
       </c>
@@ -2504,7 +2511,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" ht="33" customHeight="1" thickBot="1">
       <c r="A61" s="2" t="s">
         <v>11</v>
       </c>
@@ -2527,7 +2534,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" ht="30.75" thickBot="1">
       <c r="A62" s="33">
         <v>20</v>
       </c>
@@ -2550,7 +2557,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" ht="15.75" thickBot="1">
       <c r="A63" s="26"/>
       <c r="B63" s="20">
         <v>18</v>
@@ -2567,7 +2574,7 @@
       </c>
       <c r="G63" s="18"/>
     </row>
-    <row r="64" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" ht="15.75" thickBot="1">
       <c r="A64" s="41"/>
       <c r="B64" s="21"/>
       <c r="C64" s="20">
@@ -2582,7 +2589,7 @@
       </c>
       <c r="G64" s="18"/>
     </row>
-    <row r="65" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" ht="15.75" thickBot="1">
       <c r="A65" s="7"/>
       <c r="B65" s="8"/>
       <c r="C65" s="8"/>
@@ -2597,6 +2604,10 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A48:D48"/>
+    <mergeCell ref="A54:D54"/>
     <mergeCell ref="A60:D60"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A3:D3"/>
@@ -2605,11 +2616,8 @@
     <mergeCell ref="A21:D21"/>
     <mergeCell ref="A27:D27"/>
     <mergeCell ref="A35:D35"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="A48:D48"/>
-    <mergeCell ref="A54:D54"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <rowBreaks count="1" manualBreakCount="1">
@@ -2619,13 +2627,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
for main bot install infinity polling, fix download xlsx and xls files
</commit_message>
<xml_diff>
--- a/documents/excel_file.xlsx
+++ b/documents/excel_file.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
   <si>
     <t>Дата</t>
   </si>
@@ -42,91 +42,70 @@
     <t>Іспит</t>
   </si>
   <si>
-    <t>401-А</t>
-  </si>
-  <si>
     <t>Розклад зимової екзаменаційної сесії</t>
   </si>
   <si>
-    <t>І семестр 2020-2021  н.р.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 30.12.2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 13-30</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 25.01.2021</t>
+    <t>І семестр 2020-2021 н.р.</t>
+  </si>
+  <si>
+    <t>401-ЕП</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 26.01.2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 15-00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 08-30</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 27.01.2021</t>
+  </si>
+  <si>
+    <t>Основи товарознавства</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Васюта В.Б.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Скрильник А.С.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Підпр.та бізнес планув.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 29.01.2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 28.01.2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 01.02.2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 02.02.2021</t>
   </si>
   <si>
     <t xml:space="preserve"> 11-30</t>
   </si>
   <si>
-    <t>Філософія</t>
-  </si>
-  <si>
-    <t>Вощенко В.Ю.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 26.01.2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 15-00</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 27.01.2021</t>
-  </si>
-  <si>
-    <t>Інжен.благоус.терит.і трансп.</t>
-  </si>
-  <si>
-    <t>Савченко О.О.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 29.01.2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 01.02.2021</t>
-  </si>
-  <si>
-    <t>Основи типології</t>
-  </si>
-  <si>
-    <t>Лях В.М.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 04.02.2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 03.02.2021</t>
-  </si>
-  <si>
-    <t>Будівельна фізика</t>
-  </si>
-  <si>
-    <t>Галінська Т.А.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 08-30</t>
+    <t>Управл. персоналом</t>
+  </si>
+  <si>
+    <t>Галайда Т.О.</t>
   </si>
   <si>
     <t>Аудит.</t>
   </si>
   <si>
-    <t>Дистанційно</t>
-  </si>
-  <si>
-    <t>209-П</t>
-  </si>
-  <si>
-    <t>03-П</t>
-  </si>
-  <si>
-    <t>112-П</t>
-  </si>
-  <si>
-    <t>335-Ц</t>
+    <t>109-А</t>
+  </si>
+  <si>
+    <t>215-Ф</t>
+  </si>
+  <si>
+    <t>02-А</t>
   </si>
 </sst>
 </file>
@@ -171,7 +150,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -299,32 +278,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -355,13 +308,22 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -370,29 +332,70 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -406,17 +409,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="17" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -438,46 +434,46 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -760,7 +756,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F57"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:E1"/>
@@ -768,38 +764,39 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-    </row>
-    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
+      <c r="B3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -810,162 +807,162 @@
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
+      <c r="F5" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="15" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+      <c r="F6" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="19" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="22"/>
+      <c r="F7" s="14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="15"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="17"/>
     </row>
     <row r="9" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="F9" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="E10" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="15"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="17"/>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="18" t="s">
+      <c r="D12" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="19" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="22"/>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="17" t="s">
+      <c r="D13" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="17" t="s">
+      <c r="E13" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="19" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="17" t="s">
-        <v>24</v>
-      </c>
       <c r="F13" s="19" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="20"/>
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
@@ -973,126 +970,14 @@
       <c r="E14" s="21"/>
       <c r="F14" s="22"/>
     </row>
-    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="F15" s="19" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="F16" s="25" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="26"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="28"/>
-    </row>
-    <row r="49" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="7"/>
-      <c r="B49" s="7"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="7"/>
-      <c r="E49" s="7"/>
-    </row>
-    <row r="50" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A50" s="6"/>
-      <c r="B50" s="6"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
-    </row>
-    <row r="51" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A51" s="1"/>
-      <c r="B51" s="6"/>
-      <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="1"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="2"/>
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
-      <c r="E52" s="2"/>
-    </row>
-    <row r="53" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="3"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
-    </row>
-    <row r="54" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="4"/>
-      <c r="B54" s="5"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
-    </row>
-    <row r="55" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="3"/>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
-    </row>
-    <row r="56" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="3"/>
-      <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="3"/>
-    </row>
-    <row r="57" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="3"/>
-      <c r="B57" s="3"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
-    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="6">
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A11:F11"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="B3:D3"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="A14:F14"/>
-    <mergeCell ref="A17:F17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
fix read session for dis
</commit_message>
<xml_diff>
--- a/documents/excel_file.xlsx
+++ b/documents/excel_file.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>Дата</t>
   </si>
@@ -36,76 +36,67 @@
     <t>Викладач</t>
   </si>
   <si>
-    <t>Конс.</t>
-  </si>
-  <si>
     <t>Іспит</t>
   </si>
   <si>
+    <t>Дубіщев В.П.</t>
+  </si>
+  <si>
+    <t>Шевченко О.М.</t>
+  </si>
+  <si>
+    <t>Інформатика</t>
+  </si>
+  <si>
     <t>Розклад зимової екзаменаційної сесії</t>
   </si>
   <si>
     <t>І семестр 2020-2021 н.р.</t>
   </si>
   <si>
-    <t>401-ЕП</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 26.01.2021</t>
+    <t xml:space="preserve"> 25.01.2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11-30</t>
   </si>
   <si>
     <t xml:space="preserve"> 15-00</t>
   </si>
   <si>
-    <t xml:space="preserve"> 08-30</t>
+    <t>Щербініна С.А.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Сажко В.В.</t>
+  </si>
+  <si>
+    <t>Історія України</t>
   </si>
   <si>
     <t xml:space="preserve"> 27.01.2021</t>
   </si>
   <si>
-    <t>Основи товарознавства</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Васюта В.Б.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Скрильник А.С.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Підпр.та бізнес планув.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 29.01.2021</t>
   </si>
   <si>
-    <t xml:space="preserve"> 28.01.2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 01.02.2021</t>
+    <t>Політекономія</t>
   </si>
   <si>
     <t xml:space="preserve"> 02.02.2021</t>
   </si>
   <si>
-    <t xml:space="preserve"> 11-30</t>
-  </si>
-  <si>
-    <t>Управл. персоналом</t>
-  </si>
-  <si>
-    <t>Галайда Т.О.</t>
-  </si>
-  <si>
-    <t>Аудит.</t>
-  </si>
-  <si>
-    <t>109-А</t>
-  </si>
-  <si>
-    <t>215-Ф</t>
-  </si>
-  <si>
-    <t>02-А</t>
+    <t>Фінанси домогосподарств</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Скриль В.В.</t>
+  </si>
+  <si>
+    <t>Мікроекономіка</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 04.02.2021</t>
+  </si>
+  <si>
+    <t>101-ЕФд</t>
   </si>
 </sst>
 </file>
@@ -150,7 +141,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -204,36 +195,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -345,21 +306,6 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -382,14 +328,34 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -409,69 +375,66 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -756,7 +719,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:E1"/>
@@ -765,219 +728,193 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" customWidth="1"/>
-    <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+    </row>
+    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+    </row>
+    <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="B3" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="9" t="s">
+    </row>
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="B6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="9" t="s">
+    </row>
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="17"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="19"/>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+    </row>
+    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="17"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="19"/>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="C10" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="11"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="13"/>
+    </row>
+    <row r="12" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="11"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="13"/>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="17"/>
-    </row>
-    <row r="9" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="13" t="s">
+      <c r="C14" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="17"/>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="13" t="s">
+      <c r="D14" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" s="19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="20"/>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="22"/>
+      <c r="E14" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="14"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A14:F14"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="A11:F11"/>
+  <mergeCells count="8">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="B3:D3"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>